<commit_message>
Add dropout rates test
</commit_message>
<xml_diff>
--- a/data_prep/input_data.xlsx
+++ b/data_prep/input_data.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
     <sheet name="FertilityMotherRates" sheetId="1" r:id="rId2"/>
     <sheet name="FertilityMotherDieaseMultiplier" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Dropout" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Age</t>
   </si>
@@ -140,12 +140,93 @@
   <si>
     <t>Not sure that this is very realistic</t>
   </si>
+  <si>
+    <t>The raw values from Crhis</t>
+  </si>
+  <si>
+    <t>f.l.X0</t>
+  </si>
+  <si>
+    <t>f.l.X1</t>
+  </si>
+  <si>
+    <t>f.l.X2</t>
+  </si>
+  <si>
+    <t>f.l.X3</t>
+  </si>
+  <si>
+    <t>f.l.X4</t>
+  </si>
+  <si>
+    <t>f.l.X5</t>
+  </si>
+  <si>
+    <t>f.h.X0</t>
+  </si>
+  <si>
+    <t>f.h.X1</t>
+  </si>
+  <si>
+    <t>f.h.X2</t>
+  </si>
+  <si>
+    <t>f.h.X3</t>
+  </si>
+  <si>
+    <t>f.h.X4</t>
+  </si>
+  <si>
+    <t>f.h.X5</t>
+  </si>
+  <si>
+    <t>m.l.X0</t>
+  </si>
+  <si>
+    <t>m.l.X1</t>
+  </si>
+  <si>
+    <t>m.l.X2</t>
+  </si>
+  <si>
+    <t>m.l.X3</t>
+  </si>
+  <si>
+    <t>m.l.X4</t>
+  </si>
+  <si>
+    <t>m.l.X5</t>
+  </si>
+  <si>
+    <t>m.h.X0</t>
+  </si>
+  <si>
+    <t>m.h.X1</t>
+  </si>
+  <si>
+    <t>m.h.X2</t>
+  </si>
+  <si>
+    <t>m.h.X3</t>
+  </si>
+  <si>
+    <t>m.h.X4</t>
+  </si>
+  <si>
+    <t>m.h.X5</t>
+  </si>
+  <si>
+    <t>Round them</t>
+  </si>
+  <si>
+    <t>Now just copy and paste</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="19">
+  <numFmts count="20">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -165,6 +246,7 @@
     <numFmt numFmtId="180" formatCode="_-* #,##0.00\ _F_-;\-* #,##0.00\ _F_-;_-* &quot;-&quot;??\ _F_-;_-@_-"/>
     <numFmt numFmtId="181" formatCode="_ * #,##0_)\ _F_ ;_ * \(#,##0\)\ _F_ ;_ * &quot;-&quot;_)\ _F_ ;_ @_ "/>
     <numFmt numFmtId="182" formatCode="0.00000"/>
+    <numFmt numFmtId="183" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -411,7 +493,7 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="2" fillId="0" borderId="4" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -440,6 +522,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="182" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Bold 11" xfId="2"/>
@@ -4957,8 +5043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13436,12 +13522,2373 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="B3" s="21">
+        <v>6</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.18310192940794723</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.16784343529061829</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.22887741175993404</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.30516988234657871</v>
+      </c>
+      <c r="I3" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="J3" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="K3" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+      <c r="L3" s="23">
+        <v>5.064851212968189E-2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>6.9066152904111666E-2</v>
+      </c>
+      <c r="N3" s="23">
+        <v>9.2088203872148888E-2</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>0.18310192940794723</v>
+      </c>
+      <c r="R3" s="23">
+        <v>0.16784343529061829</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.25176515293592744</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0.30516988234657871</v>
+      </c>
+      <c r="U3" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="V3" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="W3" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+      <c r="X3" s="23">
+        <v>5.064851212968189E-2</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>7.5972768194522838E-2</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>9.2088203872148888E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="B4" s="21">
+        <v>7</v>
+      </c>
+      <c r="C4" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E4" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F4" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I4" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L4" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M4" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O4" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P4" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R4" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S4" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T4" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U4" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V4" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W4" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X4" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="B5" s="21">
+        <v>8</v>
+      </c>
+      <c r="C5" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E5" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I5" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J5" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K5" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L5" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M5" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N5" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O5" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P5" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R5" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S5" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T5" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U5" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V5" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W5" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X5" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="B6" s="21">
+        <v>9</v>
+      </c>
+      <c r="C6" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E6" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F6" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I6" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J6" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K6" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L6" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M6" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N6" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O6" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P6" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R6" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S6" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T6" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U6" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V6" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W6" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X6" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y6" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z6" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="B7" s="21">
+        <v>10</v>
+      </c>
+      <c r="C7" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D7" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E7" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F7" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I7" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J7" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K7" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L7" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M7" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N7" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O7" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P7" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R7" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S7" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T7" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U7" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V7" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W7" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X7" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y7" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z7" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="B8" s="21">
+        <v>11</v>
+      </c>
+      <c r="C8" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D8" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E8" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F8" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I8" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J8" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K8" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L8" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M8" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N8" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O8" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P8" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R8" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S8" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T8" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U8" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V8" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W8" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X8" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y8" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z8" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="B9" s="21">
+        <v>12</v>
+      </c>
+      <c r="C9" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="D9" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="E9" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="F9" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="I9" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="J9" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="K9" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="L9" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="M9" s="23">
+        <v>3.4533076452055833E-2</v>
+      </c>
+      <c r="N9" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+      <c r="O9" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="P9" s="23">
+        <v>7.6292470586644678E-2</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="R9" s="23">
+        <v>8.3921717645309146E-2</v>
+      </c>
+      <c r="S9" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="T9" s="23">
+        <v>0.15258494117328936</v>
+      </c>
+      <c r="U9" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="V9" s="23">
+        <v>2.3022050968037222E-2</v>
+      </c>
+      <c r="W9" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="X9" s="23">
+        <v>2.5324256064840945E-2</v>
+      </c>
+      <c r="Y9" s="23">
+        <v>3.7986384097261419E-2</v>
+      </c>
+      <c r="Z9" s="23">
+        <v>4.6044101936074444E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="B10" s="21">
+        <v>13</v>
+      </c>
+      <c r="C10" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="E10" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="F10" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="G10" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="I10" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="J10" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="K10" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="L10" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="M10" s="23">
+        <v>2.7626461161644668E-2</v>
+      </c>
+      <c r="N10" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+      <c r="O10" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="P10" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="R10" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="S10" s="23">
+        <v>0.10070606117437098</v>
+      </c>
+      <c r="T10" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="U10" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="V10" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="W10" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="X10" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="Y10" s="23">
+        <v>3.0389107277809135E-2</v>
+      </c>
+      <c r="Z10" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="B11" s="21">
+        <v>14</v>
+      </c>
+      <c r="C11" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="D11" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="E11" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="F11" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="G11" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="I11" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="J11" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="K11" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="L11" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="M11" s="23">
+        <v>2.7626461161644668E-2</v>
+      </c>
+      <c r="N11" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+      <c r="O11" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="P11" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="R11" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="S11" s="23">
+        <v>0.10070606117437098</v>
+      </c>
+      <c r="T11" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="U11" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="V11" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="W11" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="X11" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="Y11" s="23">
+        <v>3.0389107277809135E-2</v>
+      </c>
+      <c r="Z11" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="B12" s="21">
+        <v>15</v>
+      </c>
+      <c r="C12" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="D12" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="E12" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="G12" s="23">
+        <v>9.1550964703973614E-2</v>
+      </c>
+      <c r="H12" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="I12" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="J12" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="K12" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="L12" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="M12" s="23">
+        <v>2.7626461161644668E-2</v>
+      </c>
+      <c r="N12" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+      <c r="O12" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="P12" s="23">
+        <v>6.1033976469315743E-2</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>7.3240771763178891E-2</v>
+      </c>
+      <c r="R12" s="23">
+        <v>6.7137374116247317E-2</v>
+      </c>
+      <c r="S12" s="23">
+        <v>0.10070606117437098</v>
+      </c>
+      <c r="T12" s="23">
+        <v>0.12206795293863149</v>
+      </c>
+      <c r="U12" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="V12" s="23">
+        <v>1.841764077442978E-2</v>
+      </c>
+      <c r="W12" s="23">
+        <v>2.2101168929315736E-2</v>
+      </c>
+      <c r="X12" s="23">
+        <v>2.0259404851872758E-2</v>
+      </c>
+      <c r="Y12" s="23">
+        <v>3.0389107277809135E-2</v>
+      </c>
+      <c r="Z12" s="23">
+        <v>3.6835281548859559E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="B13" s="21">
+        <v>16</v>
+      </c>
+      <c r="C13" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.13732644705596042</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0.17165805881995053</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.22887741175993404</v>
+      </c>
+      <c r="I13" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="J13" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="K13" s="23">
+        <v>3.3151753393973596E-2</v>
+      </c>
+      <c r="L13" s="23">
+        <v>3.0389107277809132E-2</v>
+      </c>
+      <c r="M13" s="23">
+        <v>4.1439691742466998E-2</v>
+      </c>
+      <c r="N13" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="P13" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>0.13732644705596042</v>
+      </c>
+      <c r="R13" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="S13" s="23">
+        <v>0.18882386470194557</v>
+      </c>
+      <c r="T13" s="23">
+        <v>0.22887741175993404</v>
+      </c>
+      <c r="U13" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="V13" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="W13" s="23">
+        <v>3.3151753393973596E-2</v>
+      </c>
+      <c r="X13" s="23">
+        <v>3.0389107277809132E-2</v>
+      </c>
+      <c r="Y13" s="23">
+        <v>4.5583660916713696E-2</v>
+      </c>
+      <c r="Z13" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="B14" s="21">
+        <v>17</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.13732644705596042</v>
+      </c>
+      <c r="F14" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0.17165805881995053</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.22887741175993404</v>
+      </c>
+      <c r="I14" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="J14" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="K14" s="23">
+        <v>3.3151753393973596E-2</v>
+      </c>
+      <c r="L14" s="23">
+        <v>3.0389107277809132E-2</v>
+      </c>
+      <c r="M14" s="23">
+        <v>4.1439691742466998E-2</v>
+      </c>
+      <c r="N14" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+      <c r="O14" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="P14" s="23">
+        <v>0.11443870587996702</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>0.13732644705596042</v>
+      </c>
+      <c r="R14" s="23">
+        <v>0.12588257646796372</v>
+      </c>
+      <c r="S14" s="23">
+        <v>0.18882386470194557</v>
+      </c>
+      <c r="T14" s="23">
+        <v>0.22887741175993404</v>
+      </c>
+      <c r="U14" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="V14" s="23">
+        <v>2.7626461161644664E-2</v>
+      </c>
+      <c r="W14" s="23">
+        <v>3.3151753393973596E-2</v>
+      </c>
+      <c r="X14" s="23">
+        <v>3.0389107277809132E-2</v>
+      </c>
+      <c r="Y14" s="23">
+        <v>4.5583660916713696E-2</v>
+      </c>
+      <c r="Z14" s="23">
+        <v>5.5252922323289329E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="R17" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="U17" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="V17" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="W17" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="X17" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z17" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="B18" s="21">
+        <v>6</v>
+      </c>
+      <c r="C18" s="22">
+        <f>ROUND(C3, 5)</f>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="D18" s="22">
+        <f t="shared" ref="D18:Z29" si="0">ROUND(D3, 5)</f>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="F18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.16783999999999999</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22888</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.30517</v>
+      </c>
+      <c r="I18" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="J18" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="K18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.525E-2</v>
+      </c>
+      <c r="L18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.0650000000000001E-2</v>
+      </c>
+      <c r="M18" s="22">
+        <f t="shared" si="0"/>
+        <v>6.9070000000000006E-2</v>
+      </c>
+      <c r="N18" s="22">
+        <f t="shared" si="0"/>
+        <v>9.2090000000000005E-2</v>
+      </c>
+      <c r="O18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="P18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="Q18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.18310000000000001</v>
+      </c>
+      <c r="R18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.16783999999999999</v>
+      </c>
+      <c r="S18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.25176999999999999</v>
+      </c>
+      <c r="T18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.30517</v>
+      </c>
+      <c r="U18" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="V18" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="W18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.525E-2</v>
+      </c>
+      <c r="X18" s="22">
+        <f t="shared" si="0"/>
+        <v>5.0650000000000001E-2</v>
+      </c>
+      <c r="Y18" s="22">
+        <f t="shared" si="0"/>
+        <v>7.5969999999999996E-2</v>
+      </c>
+      <c r="Z18" s="22">
+        <f t="shared" si="0"/>
+        <v>9.2090000000000005E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="B19" s="21">
+        <v>7</v>
+      </c>
+      <c r="C19" s="22">
+        <f t="shared" ref="C19:R29" si="1">ROUND(C4, 5)</f>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D19" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="1"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" si="1"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="1"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="1"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I19" s="22">
+        <f t="shared" si="1"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J19" s="22">
+        <f t="shared" si="1"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K19" s="22">
+        <f t="shared" si="1"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L19" s="22">
+        <f t="shared" si="1"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M19" s="22">
+        <f t="shared" si="1"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N19" s="22">
+        <f t="shared" si="1"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O19" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P19" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q19" s="22">
+        <f t="shared" si="1"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R19" s="22">
+        <f t="shared" si="1"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S19" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T19" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U19" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V19" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W19" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X19" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y19" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z19" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="B20" s="21">
+        <v>8</v>
+      </c>
+      <c r="C20" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D20" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F20" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M20" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N20" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O20" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P20" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q20" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R20" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X20" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y20" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z20" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="B21" s="21">
+        <v>9</v>
+      </c>
+      <c r="C21" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D21" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E21" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F21" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M21" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N21" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O21" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P21" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q21" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R21" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X21" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y21" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z21" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="B22" s="21">
+        <v>10</v>
+      </c>
+      <c r="C22" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D22" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E22" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F22" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M22" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N22" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O22" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P22" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q22" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R22" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S22" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T22" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X22" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y22" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z22" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="B23" s="21">
+        <v>11</v>
+      </c>
+      <c r="C23" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D23" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F23" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H23" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M23" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N23" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O23" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P23" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q23" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R23" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S23" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T23" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X23" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y23" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z23" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="B24" s="21">
+        <v>12</v>
+      </c>
+      <c r="C24" s="22">
+        <f t="shared" si="1"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="D24" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="E24" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="F24" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="H24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="I24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="J24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="K24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="L24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="M24" s="22">
+        <f t="shared" si="0"/>
+        <v>3.4529999999999998E-2</v>
+      </c>
+      <c r="N24" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+      <c r="O24" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="P24" s="22">
+        <f t="shared" si="0"/>
+        <v>7.6289999999999997E-2</v>
+      </c>
+      <c r="Q24" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="R24" s="22">
+        <f t="shared" si="0"/>
+        <v>8.3919999999999995E-2</v>
+      </c>
+      <c r="S24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="T24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.15257999999999999</v>
+      </c>
+      <c r="U24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="V24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.3019999999999999E-2</v>
+      </c>
+      <c r="W24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="X24" s="22">
+        <f t="shared" si="0"/>
+        <v>2.5319999999999999E-2</v>
+      </c>
+      <c r="Y24" s="22">
+        <f t="shared" si="0"/>
+        <v>3.7990000000000003E-2</v>
+      </c>
+      <c r="Z24" s="22">
+        <f t="shared" si="0"/>
+        <v>4.6039999999999998E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="B25" s="21">
+        <v>13</v>
+      </c>
+      <c r="C25" s="22">
+        <f t="shared" si="1"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="D25" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="E25" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="F25" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="H25" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="I25" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="J25" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="K25" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="L25" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="M25" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="N25" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+      <c r="O25" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="P25" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="Q25" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="R25" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="S25" s="22">
+        <f t="shared" si="0"/>
+        <v>0.10070999999999999</v>
+      </c>
+      <c r="T25" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="U25" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="V25" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="W25" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="X25" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="Y25" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="Z25" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="B26" s="21">
+        <v>14</v>
+      </c>
+      <c r="C26" s="22">
+        <f t="shared" si="1"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="D26" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="E26" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="F26" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="H26" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="I26" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="J26" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="K26" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="L26" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="M26" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="N26" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+      <c r="O26" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="P26" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="Q26" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="R26" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="S26" s="22">
+        <f t="shared" si="0"/>
+        <v>0.10070999999999999</v>
+      </c>
+      <c r="T26" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="U26" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="V26" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="W26" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="X26" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="Y26" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="Z26" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="B27" s="21">
+        <v>15</v>
+      </c>
+      <c r="C27" s="22">
+        <f t="shared" si="1"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="D27" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="E27" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="F27" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="0"/>
+        <v>9.1550000000000006E-2</v>
+      </c>
+      <c r="H27" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="I27" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="J27" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="K27" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="L27" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="M27" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="N27" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+      <c r="O27" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="P27" s="22">
+        <f t="shared" si="0"/>
+        <v>6.1030000000000001E-2</v>
+      </c>
+      <c r="Q27" s="22">
+        <f t="shared" si="0"/>
+        <v>7.324E-2</v>
+      </c>
+      <c r="R27" s="22">
+        <f t="shared" si="0"/>
+        <v>6.7140000000000005E-2</v>
+      </c>
+      <c r="S27" s="22">
+        <f t="shared" si="0"/>
+        <v>0.10070999999999999</v>
+      </c>
+      <c r="T27" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12207</v>
+      </c>
+      <c r="U27" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="V27" s="22">
+        <f t="shared" si="0"/>
+        <v>1.8419999999999999E-2</v>
+      </c>
+      <c r="W27" s="22">
+        <f t="shared" si="0"/>
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="X27" s="22">
+        <f t="shared" si="0"/>
+        <v>2.026E-2</v>
+      </c>
+      <c r="Y27" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="Z27" s="22">
+        <f t="shared" si="0"/>
+        <v>3.6839999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="B28" s="21">
+        <v>16</v>
+      </c>
+      <c r="C28" s="22">
+        <f t="shared" si="1"/>
+        <v>0.11444</v>
+      </c>
+      <c r="D28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="E28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.13733000000000001</v>
+      </c>
+      <c r="F28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.17166000000000001</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22888</v>
+      </c>
+      <c r="I28" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="J28" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="K28" s="22">
+        <f t="shared" si="0"/>
+        <v>3.3149999999999999E-2</v>
+      </c>
+      <c r="L28" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="M28" s="22">
+        <f t="shared" si="0"/>
+        <v>4.1439999999999998E-2</v>
+      </c>
+      <c r="N28" s="22">
+        <f t="shared" si="0"/>
+        <v>5.525E-2</v>
+      </c>
+      <c r="O28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="P28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="Q28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.13733000000000001</v>
+      </c>
+      <c r="R28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="S28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.18881999999999999</v>
+      </c>
+      <c r="T28" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22888</v>
+      </c>
+      <c r="U28" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="V28" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="W28" s="22">
+        <f t="shared" si="0"/>
+        <v>3.3149999999999999E-2</v>
+      </c>
+      <c r="X28" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="Y28" s="22">
+        <f t="shared" si="0"/>
+        <v>4.5580000000000002E-2</v>
+      </c>
+      <c r="Z28" s="22">
+        <f t="shared" si="0"/>
+        <v>5.525E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="B29" s="21">
+        <v>17</v>
+      </c>
+      <c r="C29" s="22">
+        <f t="shared" si="1"/>
+        <v>0.11444</v>
+      </c>
+      <c r="D29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="E29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.13733000000000001</v>
+      </c>
+      <c r="F29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.17166000000000001</v>
+      </c>
+      <c r="H29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22888</v>
+      </c>
+      <c r="I29" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="J29" s="22">
+        <f t="shared" si="0"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="K29" s="22">
+        <f t="shared" si="0"/>
+        <v>3.3149999999999999E-2</v>
+      </c>
+      <c r="L29" s="22">
+        <f t="shared" si="0"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="M29" s="22">
+        <f t="shared" si="0"/>
+        <v>4.1439999999999998E-2</v>
+      </c>
+      <c r="N29" s="22">
+        <f t="shared" si="0"/>
+        <v>5.525E-2</v>
+      </c>
+      <c r="O29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="P29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.11444</v>
+      </c>
+      <c r="Q29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.13733000000000001</v>
+      </c>
+      <c r="R29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12587999999999999</v>
+      </c>
+      <c r="S29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.18881999999999999</v>
+      </c>
+      <c r="T29" s="22">
+        <f t="shared" si="0"/>
+        <v>0.22888</v>
+      </c>
+      <c r="U29" s="22">
+        <f t="shared" ref="U29:Z29" si="2">ROUND(U14, 5)</f>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="V29" s="22">
+        <f t="shared" si="2"/>
+        <v>2.7629999999999998E-2</v>
+      </c>
+      <c r="W29" s="22">
+        <f t="shared" si="2"/>
+        <v>3.3149999999999999E-2</v>
+      </c>
+      <c r="X29" s="22">
+        <f t="shared" si="2"/>
+        <v>3.039E-2</v>
+      </c>
+      <c r="Y29" s="22">
+        <f t="shared" si="2"/>
+        <v>4.5580000000000002E-2</v>
+      </c>
+      <c r="Z29" s="22">
+        <f t="shared" si="2"/>
+        <v>5.525E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add real AbusedDepression Probabilities
</commit_message>
<xml_diff>
--- a/data_prep/input_data.xlsx
+++ b/data_prep/input_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -12,9 +12,10 @@
     <sheet name="FertilityMotherDieaseMultiplier" sheetId="2" r:id="rId3"/>
     <sheet name="Dropout" sheetId="3" r:id="rId4"/>
     <sheet name="Abuse" sheetId="5" r:id="rId5"/>
+    <sheet name="Abused Depression" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="CurrYear">[1]Results!$B$3</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
   <si>
     <t>Age</t>
   </si>
@@ -498,7 +499,7 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="2" fillId="0" borderId="4" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -535,6 +536,8 @@
     <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Bold 11" xfId="2"/>
@@ -15906,8 +15909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14:Z20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17335,4 +17338,1459 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="26"/>
+      <c r="B2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="26"/>
+      <c r="B3" s="28">
+        <v>12</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.13072032357909907</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.13072032357909907</v>
+      </c>
+      <c r="E3" s="23">
+        <v>8.7781920090155188E-2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>3.5112768036062079E-2</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.17556384018031038</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.19002206560710103</v>
+      </c>
+      <c r="I3" s="23">
+        <v>5.9635640495214338E-2</v>
+      </c>
+      <c r="J3" s="23">
+        <v>5.9635640495214338E-2</v>
+      </c>
+      <c r="K3" s="23">
+        <v>4.1293421303029307E-2</v>
+      </c>
+      <c r="L3" s="23">
+        <v>1.6517368521211724E-2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>8.2586842606058614E-2</v>
+      </c>
+      <c r="N3" s="23">
+        <v>9.027636511993109E-2</v>
+      </c>
+      <c r="O3" s="23">
+        <v>8.8609827724222198E-2</v>
+      </c>
+      <c r="P3" s="23">
+        <v>8.8609827724222198E-2</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>6.0588804753311985E-2</v>
+      </c>
+      <c r="R3" s="23">
+        <v>2.4235521901324796E-2</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.12117760950662397</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0.13191776806942238</v>
+      </c>
+      <c r="U3" s="23">
+        <v>3.9258168697638492E-2</v>
+      </c>
+      <c r="V3" s="23">
+        <v>3.9258168697638492E-2</v>
+      </c>
+      <c r="W3" s="23">
+        <v>2.7427136262616711E-2</v>
+      </c>
+      <c r="X3" s="23">
+        <v>1.0970854505046685E-2</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>5.4854272525233422E-2</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>6.0138786840652658E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="26"/>
+      <c r="B4" s="28">
+        <v>13</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.14826936823900039</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.14826936823900039</v>
+      </c>
+      <c r="E4" s="23">
+        <v>9.6584553235701504E-2</v>
+      </c>
+      <c r="F4" s="23">
+        <v>3.8633821294280606E-2</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.19316910647140301</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.20749853238479582</v>
+      </c>
+      <c r="I4" s="23">
+        <v>6.8489779559944258E-2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>6.8489779559944258E-2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>4.6094105663264641E-2</v>
+      </c>
+      <c r="L4" s="23">
+        <v>1.8437642265305858E-2</v>
+      </c>
+      <c r="M4" s="23">
+        <v>9.2188211326529282E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <v>0.10008586033603298</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0.10124841846462271</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0.10124841846462271</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>6.7226009388458755E-2</v>
+      </c>
+      <c r="R4" s="23">
+        <v>2.6890403755383502E-2</v>
+      </c>
+      <c r="S4" s="23">
+        <v>0.13445201877691751</v>
+      </c>
+      <c r="T4" s="23">
+        <v>0.14532003544507888</v>
+      </c>
+      <c r="U4" s="23">
+        <v>4.5822291862324768E-2</v>
+      </c>
+      <c r="V4" s="23">
+        <v>4.5822291862324768E-2</v>
+      </c>
+      <c r="W4" s="23">
+        <v>3.1816237516487322E-2</v>
+      </c>
+      <c r="X4" s="23">
+        <v>1.272649500659493E-2</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>6.3632475032974645E-2</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>6.9647157565001047E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="26"/>
+      <c r="B5" s="28">
+        <v>14</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0.16766160955157292</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.16766160955157292</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.10837134869662345</v>
+      </c>
+      <c r="F5" s="23">
+        <v>4.3348539478649382E-2</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.21674269739324689</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.23224687387015924</v>
+      </c>
+      <c r="I5" s="23">
+        <v>7.8535874423254479E-2</v>
+      </c>
+      <c r="J5" s="23">
+        <v>7.8535874423254479E-2</v>
+      </c>
+      <c r="K5" s="23">
+        <v>5.2635544194574398E-2</v>
+      </c>
+      <c r="L5" s="23">
+        <v>2.1054217677829761E-2</v>
+      </c>
+      <c r="M5" s="23">
+        <v>0.1052710883891488</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0.11413144566820385</v>
+      </c>
+      <c r="O5" s="23">
+        <v>0.11543364732735795</v>
+      </c>
+      <c r="P5" s="23">
+        <v>0.11543364732735795</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>7.6201467871442996E-2</v>
+      </c>
+      <c r="R5" s="23">
+        <v>3.0480587148577199E-2</v>
+      </c>
+      <c r="S5" s="23">
+        <v>0.15240293574288599</v>
+      </c>
+      <c r="T5" s="23">
+        <v>0.16441078039090012</v>
+      </c>
+      <c r="U5" s="23">
+        <v>5.332907393622692E-2</v>
+      </c>
+      <c r="V5" s="23">
+        <v>5.332907393622692E-2</v>
+      </c>
+      <c r="W5" s="23">
+        <v>3.6809012415341527E-2</v>
+      </c>
+      <c r="X5" s="23">
+        <v>1.4723604966136611E-2</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>7.3618024830683054E-2</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>8.0443889665049603E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="26"/>
+      <c r="B6" s="28">
+        <v>15</v>
+      </c>
+      <c r="C6" s="23">
+        <v>0.18895348428302433</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.18895348428302433</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.12110418052669357</v>
+      </c>
+      <c r="F6" s="23">
+        <v>4.8441672210677432E-2</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.24220836105338714</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0.25884472561381183</v>
+      </c>
+      <c r="I6" s="23">
+        <v>8.9896510804592988E-2</v>
+      </c>
+      <c r="J6" s="23">
+        <v>8.9896510804592988E-2</v>
+      </c>
+      <c r="K6" s="23">
+        <v>5.9967709986047536E-2</v>
+      </c>
+      <c r="L6" s="23">
+        <v>2.3987083994419015E-2</v>
+      </c>
+      <c r="M6" s="23">
+        <v>0.11993541997209507</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0.12982872201365486</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0.13128015246148522</v>
+      </c>
+      <c r="P6" s="23">
+        <v>0.13128015246148522</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>8.6106063047996562E-2</v>
+      </c>
+      <c r="R6" s="23">
+        <v>3.4442425219198623E-2</v>
+      </c>
+      <c r="S6" s="23">
+        <v>0.17221212609599312</v>
+      </c>
+      <c r="T6" s="23">
+        <v>0.18539419793419482</v>
+      </c>
+      <c r="U6" s="23">
+        <v>6.189465567146632E-2</v>
+      </c>
+      <c r="V6" s="23">
+        <v>6.189465567146632E-2</v>
+      </c>
+      <c r="W6" s="23">
+        <v>4.2471577296019893E-2</v>
+      </c>
+      <c r="X6" s="23">
+        <v>1.6988630918407958E-2</v>
+      </c>
+      <c r="Y6" s="23">
+        <v>8.4943154592039785E-2</v>
+      </c>
+      <c r="Z6" s="23">
+        <v>9.266408977527113E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="26"/>
+      <c r="B7" s="28">
+        <v>16</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0.21216686250271777</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0.21216686250271777</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.13474352577547533</v>
+      </c>
+      <c r="F7" s="23">
+        <v>5.389741031019013E-2</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.26948705155095065</v>
+      </c>
+      <c r="H7" s="23">
+        <v>0.2871797599944742</v>
+      </c>
+      <c r="I7" s="23">
+        <v>0.10269543582069027</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0.10269543582069027</v>
+      </c>
+      <c r="K7" s="23">
+        <v>6.8146365011634014E-2</v>
+      </c>
+      <c r="L7" s="23">
+        <v>2.7258546004653605E-2</v>
+      </c>
+      <c r="M7" s="23">
+        <v>0.13629273002326803</v>
+      </c>
+      <c r="N7" s="23">
+        <v>0.14728095246135559</v>
+      </c>
+      <c r="O7" s="23">
+        <v>0.14888982889461763</v>
+      </c>
+      <c r="P7" s="23">
+        <v>0.14888982889461763</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>9.6964524654654896E-2</v>
+      </c>
+      <c r="R7" s="23">
+        <v>3.8785809861861961E-2</v>
+      </c>
+      <c r="S7" s="23">
+        <v>0.19392904930930979</v>
+      </c>
+      <c r="T7" s="23">
+        <v>0.2082982549266541</v>
+      </c>
+      <c r="U7" s="23">
+        <v>7.1643399983750369E-2</v>
+      </c>
+      <c r="V7" s="23">
+        <v>7.1643399983750369E-2</v>
+      </c>
+      <c r="W7" s="23">
+        <v>4.8872104639166122E-2</v>
+      </c>
+      <c r="X7" s="23">
+        <v>1.9548841855666452E-2</v>
+      </c>
+      <c r="Y7" s="23">
+        <v>9.7744209278332245E-2</v>
+      </c>
+      <c r="Z7" s="23">
+        <v>0.1064450605052412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="26"/>
+      <c r="B8" s="28">
+        <v>17</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.23728141398439886</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.23728141398439886</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.14922260757988282</v>
+      </c>
+      <c r="F8" s="23">
+        <v>5.9689043031953132E-2</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.29844521515976563</v>
+      </c>
+      <c r="H8" s="23">
+        <v>0.31708368915278728</v>
+      </c>
+      <c r="I8" s="23">
+        <v>0.11705373594432186</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0.11705373594432186</v>
+      </c>
+      <c r="K8" s="23">
+        <v>7.721994858392113E-2</v>
+      </c>
+      <c r="L8" s="23">
+        <v>3.0887979433568455E-2</v>
+      </c>
+      <c r="M8" s="23">
+        <v>0.15443989716784226</v>
+      </c>
+      <c r="N8" s="23">
+        <v>0.16657252414397133</v>
+      </c>
+      <c r="O8" s="23">
+        <v>0.16834507260725676</v>
+      </c>
+      <c r="P8" s="23">
+        <v>0.16834507260725676</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>0.10878343347914121</v>
+      </c>
+      <c r="R8" s="23">
+        <v>4.3513373391656486E-2</v>
+      </c>
+      <c r="S8" s="23">
+        <v>0.21756686695828242</v>
+      </c>
+      <c r="T8" s="23">
+        <v>0.23310990551610464</v>
+      </c>
+      <c r="U8" s="23">
+        <v>8.2706478261945063E-2</v>
+      </c>
+      <c r="V8" s="23">
+        <v>8.2706478261945063E-2</v>
+      </c>
+      <c r="W8" s="23">
+        <v>5.6079173180596985E-2</v>
+      </c>
+      <c r="X8" s="23">
+        <v>2.2431669272238795E-2</v>
+      </c>
+      <c r="Y8" s="23">
+        <v>0.11215834636119397</v>
+      </c>
+      <c r="Z8" s="23">
+        <v>0.12192234785265216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="26"/>
+      <c r="B9" s="28">
+        <v>18</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.2642279024146969</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.2642279024146969</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.16444652392789583</v>
+      </c>
+      <c r="F9" s="23">
+        <v>6.5778609571158331E-2</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.32889304785579165</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.34833259726949661</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0.1330849768166428</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0.1330849768166428</v>
+      </c>
+      <c r="K9" s="23">
+        <v>8.7226075452098414E-2</v>
+      </c>
+      <c r="L9" s="23">
+        <v>3.4890430180839364E-2</v>
+      </c>
+      <c r="M9" s="23">
+        <v>0.17445215090419683</v>
+      </c>
+      <c r="N9" s="23">
+        <v>0.1877615070306955</v>
+      </c>
+      <c r="O9" s="23">
+        <v>0.18970128807672451</v>
+      </c>
+      <c r="P9" s="23">
+        <v>0.18970128807672451</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>0.12154747348797017</v>
+      </c>
+      <c r="R9" s="23">
+        <v>4.8618989395188071E-2</v>
+      </c>
+      <c r="S9" s="23">
+        <v>0.24309494697594033</v>
+      </c>
+      <c r="T9" s="23">
+        <v>0.25976818131547708</v>
+      </c>
+      <c r="U9" s="23">
+        <v>9.5219683807686056E-2</v>
+      </c>
+      <c r="V9" s="23">
+        <v>9.5219683807686056E-2</v>
+      </c>
+      <c r="W9" s="23">
+        <v>6.4159579280315654E-2</v>
+      </c>
+      <c r="X9" s="23">
+        <v>2.5663831712126262E-2</v>
+      </c>
+      <c r="Y9" s="23">
+        <v>0.12831915856063131</v>
+      </c>
+      <c r="Z9" s="23">
+        <v>0.13922465565303327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="26"/>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="26"/>
+      <c r="B12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="U12" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="V12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="X12" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y12" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z12" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="26"/>
+      <c r="B13" s="29">
+        <v>12</v>
+      </c>
+      <c r="C13" s="23">
+        <f>ROUND(C3,5)</f>
+        <v>0.13072</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" ref="D13:Z19" si="0">ROUND(D3,5)</f>
+        <v>0.13072</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>8.7779999999999997E-2</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="0"/>
+        <v>3.5110000000000002E-2</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17555999999999999</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19001999999999999</v>
+      </c>
+      <c r="I13" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9639999999999999E-2</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9639999999999999E-2</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="0"/>
+        <v>4.129E-2</v>
+      </c>
+      <c r="L13" s="23">
+        <f t="shared" si="0"/>
+        <v>1.652E-2</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2589999999999997E-2</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="0"/>
+        <v>9.0279999999999999E-2</v>
+      </c>
+      <c r="O13" s="23">
+        <f t="shared" si="0"/>
+        <v>8.8609999999999994E-2</v>
+      </c>
+      <c r="P13" s="23">
+        <f t="shared" si="0"/>
+        <v>8.8609999999999994E-2</v>
+      </c>
+      <c r="Q13" s="23">
+        <f t="shared" si="0"/>
+        <v>6.0589999999999998E-2</v>
+      </c>
+      <c r="R13" s="23">
+        <f t="shared" si="0"/>
+        <v>2.4240000000000001E-2</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12118</v>
+      </c>
+      <c r="T13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13192000000000001</v>
+      </c>
+      <c r="U13" s="23">
+        <f t="shared" si="0"/>
+        <v>3.9260000000000003E-2</v>
+      </c>
+      <c r="V13" s="23">
+        <f t="shared" si="0"/>
+        <v>3.9260000000000003E-2</v>
+      </c>
+      <c r="W13" s="23">
+        <f t="shared" si="0"/>
+        <v>2.743E-2</v>
+      </c>
+      <c r="X13" s="23">
+        <f t="shared" si="0"/>
+        <v>1.0970000000000001E-2</v>
+      </c>
+      <c r="Y13" s="23">
+        <f t="shared" si="0"/>
+        <v>5.4850000000000003E-2</v>
+      </c>
+      <c r="Z13" s="23">
+        <f t="shared" si="0"/>
+        <v>6.0139999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="26"/>
+      <c r="B14" s="29">
+        <v>13</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" ref="C14:R19" si="1">ROUND(C4,5)</f>
+        <v>0.14827000000000001</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.14827000000000001</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="1"/>
+        <v>9.6579999999999999E-2</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>3.8629999999999998E-2</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.19317000000000001</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="1"/>
+        <v>6.8489999999999995E-2</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="1"/>
+        <v>6.8489999999999995E-2</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="1"/>
+        <v>4.6089999999999999E-2</v>
+      </c>
+      <c r="L14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8440000000000002E-2</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="1"/>
+        <v>9.2189999999999994E-2</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10009</v>
+      </c>
+      <c r="O14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10125000000000001</v>
+      </c>
+      <c r="P14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10125000000000001</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="1"/>
+        <v>6.7229999999999998E-2</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.6890000000000001E-2</v>
+      </c>
+      <c r="S14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13444999999999999</v>
+      </c>
+      <c r="T14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14532</v>
+      </c>
+      <c r="U14" s="23">
+        <f t="shared" si="0"/>
+        <v>4.582E-2</v>
+      </c>
+      <c r="V14" s="23">
+        <f t="shared" si="0"/>
+        <v>4.582E-2</v>
+      </c>
+      <c r="W14" s="23">
+        <f t="shared" si="0"/>
+        <v>3.1820000000000001E-2</v>
+      </c>
+      <c r="X14" s="23">
+        <f t="shared" si="0"/>
+        <v>1.273E-2</v>
+      </c>
+      <c r="Y14" s="23">
+        <f t="shared" si="0"/>
+        <v>6.3630000000000006E-2</v>
+      </c>
+      <c r="Z14" s="23">
+        <f t="shared" si="0"/>
+        <v>6.9650000000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="26"/>
+      <c r="B15" s="29">
+        <v>14</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="1"/>
+        <v>0.16766</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16766</v>
+      </c>
+      <c r="E15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10836999999999999</v>
+      </c>
+      <c r="F15" s="23">
+        <f t="shared" si="0"/>
+        <v>4.335E-2</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21673999999999999</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23225000000000001</v>
+      </c>
+      <c r="I15" s="23">
+        <f t="shared" si="0"/>
+        <v>7.8539999999999999E-2</v>
+      </c>
+      <c r="J15" s="23">
+        <f t="shared" si="0"/>
+        <v>7.8539999999999999E-2</v>
+      </c>
+      <c r="K15" s="23">
+        <f t="shared" si="0"/>
+        <v>5.2639999999999999E-2</v>
+      </c>
+      <c r="L15" s="23">
+        <f t="shared" si="0"/>
+        <v>2.1049999999999999E-2</v>
+      </c>
+      <c r="M15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10527</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11413</v>
+      </c>
+      <c r="O15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11543</v>
+      </c>
+      <c r="P15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11543</v>
+      </c>
+      <c r="Q15" s="23">
+        <f t="shared" si="0"/>
+        <v>7.6200000000000004E-2</v>
+      </c>
+      <c r="R15" s="23">
+        <f t="shared" si="0"/>
+        <v>3.048E-2</v>
+      </c>
+      <c r="S15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15240000000000001</v>
+      </c>
+      <c r="T15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16441</v>
+      </c>
+      <c r="U15" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3330000000000002E-2</v>
+      </c>
+      <c r="V15" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3330000000000002E-2</v>
+      </c>
+      <c r="W15" s="23">
+        <f t="shared" si="0"/>
+        <v>3.6810000000000002E-2</v>
+      </c>
+      <c r="X15" s="23">
+        <f t="shared" si="0"/>
+        <v>1.472E-2</v>
+      </c>
+      <c r="Y15" s="23">
+        <f t="shared" si="0"/>
+        <v>7.3620000000000005E-2</v>
+      </c>
+      <c r="Z15" s="23">
+        <f t="shared" si="0"/>
+        <v>8.0439999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="26"/>
+      <c r="B16" s="29">
+        <v>15</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" si="1"/>
+        <v>0.18895000000000001</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18895000000000001</v>
+      </c>
+      <c r="E16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1211</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" si="0"/>
+        <v>4.8439999999999997E-2</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.24221000000000001</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25884000000000001</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9899999999999994E-2</v>
+      </c>
+      <c r="J16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9899999999999994E-2</v>
+      </c>
+      <c r="K16" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9970000000000002E-2</v>
+      </c>
+      <c r="L16" s="23">
+        <f t="shared" si="0"/>
+        <v>2.3990000000000001E-2</v>
+      </c>
+      <c r="M16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11994</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12983</v>
+      </c>
+      <c r="O16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13128000000000001</v>
+      </c>
+      <c r="P16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13128000000000001</v>
+      </c>
+      <c r="Q16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.6110000000000006E-2</v>
+      </c>
+      <c r="R16" s="23">
+        <f t="shared" si="0"/>
+        <v>3.4439999999999998E-2</v>
+      </c>
+      <c r="S16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17221</v>
+      </c>
+      <c r="T16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18539</v>
+      </c>
+      <c r="U16" s="23">
+        <f t="shared" si="0"/>
+        <v>6.1890000000000001E-2</v>
+      </c>
+      <c r="V16" s="23">
+        <f t="shared" si="0"/>
+        <v>6.1890000000000001E-2</v>
+      </c>
+      <c r="W16" s="23">
+        <f t="shared" si="0"/>
+        <v>4.2470000000000001E-2</v>
+      </c>
+      <c r="X16" s="23">
+        <f t="shared" si="0"/>
+        <v>1.6990000000000002E-2</v>
+      </c>
+      <c r="Y16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.4940000000000002E-2</v>
+      </c>
+      <c r="Z16" s="23">
+        <f t="shared" si="0"/>
+        <v>9.2660000000000006E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" s="26"/>
+      <c r="B17" s="29">
+        <v>16</v>
+      </c>
+      <c r="C17" s="23">
+        <f t="shared" si="1"/>
+        <v>0.21217</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21217</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13474</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.26949000000000001</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28717999999999999</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1027</v>
+      </c>
+      <c r="J17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1027</v>
+      </c>
+      <c r="K17" s="23">
+        <f t="shared" si="0"/>
+        <v>6.8150000000000002E-2</v>
+      </c>
+      <c r="L17" s="23">
+        <f t="shared" si="0"/>
+        <v>2.726E-2</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13628999999999999</v>
+      </c>
+      <c r="N17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14727999999999999</v>
+      </c>
+      <c r="O17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14888999999999999</v>
+      </c>
+      <c r="P17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14888999999999999</v>
+      </c>
+      <c r="Q17" s="23">
+        <f t="shared" si="0"/>
+        <v>9.6960000000000005E-2</v>
+      </c>
+      <c r="R17" s="23">
+        <f t="shared" si="0"/>
+        <v>3.8789999999999998E-2</v>
+      </c>
+      <c r="S17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19392999999999999</v>
+      </c>
+      <c r="T17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="U17" s="23">
+        <f t="shared" si="0"/>
+        <v>7.1639999999999995E-2</v>
+      </c>
+      <c r="V17" s="23">
+        <f t="shared" si="0"/>
+        <v>7.1639999999999995E-2</v>
+      </c>
+      <c r="W17" s="23">
+        <f t="shared" si="0"/>
+        <v>4.8869999999999997E-2</v>
+      </c>
+      <c r="X17" s="23">
+        <f t="shared" si="0"/>
+        <v>1.9550000000000001E-2</v>
+      </c>
+      <c r="Y17" s="23">
+        <f t="shared" si="0"/>
+        <v>9.7739999999999994E-2</v>
+      </c>
+      <c r="Z17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="26"/>
+      <c r="B18" s="29">
+        <v>17</v>
+      </c>
+      <c r="C18" s="23">
+        <f t="shared" si="1"/>
+        <v>0.23727999999999999</v>
+      </c>
+      <c r="D18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23727999999999999</v>
+      </c>
+      <c r="E18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14921999999999999</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" si="0"/>
+        <v>5.969E-2</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.29844999999999999</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31707999999999997</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11705</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11705</v>
+      </c>
+      <c r="K18" s="23">
+        <f t="shared" si="0"/>
+        <v>7.7219999999999997E-2</v>
+      </c>
+      <c r="L18" s="23">
+        <f t="shared" si="0"/>
+        <v>3.0890000000000001E-2</v>
+      </c>
+      <c r="M18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15443999999999999</v>
+      </c>
+      <c r="N18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16657</v>
+      </c>
+      <c r="O18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16835</v>
+      </c>
+      <c r="P18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16835</v>
+      </c>
+      <c r="Q18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10878</v>
+      </c>
+      <c r="R18" s="23">
+        <f t="shared" si="0"/>
+        <v>4.351E-2</v>
+      </c>
+      <c r="S18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21757000000000001</v>
+      </c>
+      <c r="T18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23311000000000001</v>
+      </c>
+      <c r="U18" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2710000000000006E-2</v>
+      </c>
+      <c r="V18" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2710000000000006E-2</v>
+      </c>
+      <c r="W18" s="23">
+        <f t="shared" si="0"/>
+        <v>5.6079999999999998E-2</v>
+      </c>
+      <c r="X18" s="23">
+        <f t="shared" si="0"/>
+        <v>2.2429999999999999E-2</v>
+      </c>
+      <c r="Y18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11216</v>
+      </c>
+      <c r="Z18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="26"/>
+      <c r="B19" s="29">
+        <v>18</v>
+      </c>
+      <c r="C19" s="23">
+        <f t="shared" si="1"/>
+        <v>0.26423000000000002</v>
+      </c>
+      <c r="D19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.26423000000000002</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16445000000000001</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="0"/>
+        <v>6.5780000000000005E-2</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.32889000000000002</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.34832999999999997</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13308</v>
+      </c>
+      <c r="J19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13308</v>
+      </c>
+      <c r="K19" s="23">
+        <f t="shared" si="0"/>
+        <v>8.7230000000000002E-2</v>
+      </c>
+      <c r="L19" s="23">
+        <f t="shared" si="0"/>
+        <v>3.4889999999999997E-2</v>
+      </c>
+      <c r="M19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17444999999999999</v>
+      </c>
+      <c r="N19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18776000000000001</v>
+      </c>
+      <c r="O19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18970000000000001</v>
+      </c>
+      <c r="P19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18970000000000001</v>
+      </c>
+      <c r="Q19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12155000000000001</v>
+      </c>
+      <c r="R19" s="23">
+        <f t="shared" si="0"/>
+        <v>4.8619999999999997E-2</v>
+      </c>
+      <c r="S19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.24309</v>
+      </c>
+      <c r="T19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25977</v>
+      </c>
+      <c r="U19" s="23">
+        <f t="shared" si="0"/>
+        <v>9.5219999999999999E-2</v>
+      </c>
+      <c r="V19" s="23">
+        <f t="shared" si="0"/>
+        <v>9.5219999999999999E-2</v>
+      </c>
+      <c r="W19" s="23">
+        <f t="shared" si="0"/>
+        <v>6.4159999999999995E-2</v>
+      </c>
+      <c r="X19" s="23">
+        <f t="shared" si="0"/>
+        <v>2.5659999999999999E-2</v>
+      </c>
+      <c r="Y19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12831999999999999</v>
+      </c>
+      <c r="Z19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13922000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="26"/>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="26"/>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add real NotAbusedDepression Probabilities
</commit_message>
<xml_diff>
--- a/data_prep/input_data.xlsx
+++ b/data_prep/input_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -12,10 +12,11 @@
     <sheet name="FertilityMotherDieaseMultiplier" sheetId="2" r:id="rId3"/>
     <sheet name="Dropout" sheetId="3" r:id="rId4"/>
     <sheet name="Abuse" sheetId="5" r:id="rId5"/>
-    <sheet name="Abused Depression" sheetId="6" r:id="rId6"/>
+    <sheet name="Not Abused Depression" sheetId="6" r:id="rId6"/>
+    <sheet name="Abused Depression" sheetId="7" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="CurrYear">[1]Results!$B$3</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="57">
   <si>
     <t>Age</t>
   </si>
@@ -499,7 +500,7 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="2" fillId="0" borderId="4" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -537,6 +538,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="28">
@@ -17344,8 +17348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18793,4 +18797,1459 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13:Z19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30">
+        <v>12</v>
+      </c>
+      <c r="C3" s="31">
+        <v>0.29550584974001159</v>
+      </c>
+      <c r="D3" s="31">
+        <v>0.29550584974001159</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0.18447309438766898</v>
+      </c>
+      <c r="F3" s="31">
+        <v>7.3789237755067599E-2</v>
+      </c>
+      <c r="G3" s="31">
+        <v>0.36894618877533797</v>
+      </c>
+      <c r="H3" s="31">
+        <v>0.39087881343329189</v>
+      </c>
+      <c r="I3" s="31">
+        <v>0.15115219942802108</v>
+      </c>
+      <c r="J3" s="31">
+        <v>0.15115219942802108</v>
+      </c>
+      <c r="K3" s="31">
+        <v>9.9606279074667695E-2</v>
+      </c>
+      <c r="L3" s="31">
+        <v>3.9842511629867079E-2</v>
+      </c>
+      <c r="M3" s="31">
+        <v>0.19921255814933539</v>
+      </c>
+      <c r="N3" s="31">
+        <v>0.21460746499850836</v>
+      </c>
+      <c r="O3" s="31">
+        <v>0.2140482687790832</v>
+      </c>
+      <c r="P3" s="31">
+        <v>0.2140482687790832</v>
+      </c>
+      <c r="Q3" s="31">
+        <v>0.13773069646100677</v>
+      </c>
+      <c r="R3" s="31">
+        <v>5.5092278584402715E-2</v>
+      </c>
+      <c r="S3" s="31">
+        <v>0.27546139292201355</v>
+      </c>
+      <c r="T3" s="31">
+        <v>0.29453229660845154</v>
+      </c>
+      <c r="U3" s="31">
+        <v>0.1030604304862867</v>
+      </c>
+      <c r="V3" s="31">
+        <v>0.1030604304862867</v>
+      </c>
+      <c r="W3" s="31">
+        <v>6.9184594675518768E-2</v>
+      </c>
+      <c r="X3" s="31">
+        <v>2.767383787020751E-2</v>
+      </c>
+      <c r="Y3" s="31">
+        <v>0.13836918935103754</v>
+      </c>
+      <c r="Z3" s="31">
+        <v>0.14995774555657526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="29"/>
+      <c r="B4" s="30">
+        <v>13</v>
+      </c>
+      <c r="C4" s="31">
+        <v>0.30992924849221043</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0.30992924849221043</v>
+      </c>
+      <c r="E4" s="31">
+        <v>0.1895566420334292</v>
+      </c>
+      <c r="F4" s="31">
+        <v>7.5822656813371692E-2</v>
+      </c>
+      <c r="G4" s="31">
+        <v>0.3791132840668584</v>
+      </c>
+      <c r="H4" s="31">
+        <v>0.39944588176607454</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0.16187209217418533</v>
+      </c>
+      <c r="J4" s="31">
+        <v>0.16187209217418533</v>
+      </c>
+      <c r="K4" s="31">
+        <v>0.10487158957596845</v>
+      </c>
+      <c r="L4" s="31">
+        <v>4.1948635830387382E-2</v>
+      </c>
+      <c r="M4" s="31">
+        <v>0.20974317915193691</v>
+      </c>
+      <c r="N4" s="31">
+        <v>0.22491130127072356</v>
+      </c>
+      <c r="O4" s="31">
+        <v>0.2271126340374299</v>
+      </c>
+      <c r="P4" s="31">
+        <v>0.2271126340374299</v>
+      </c>
+      <c r="Q4" s="31">
+        <v>0.14339429832113498</v>
+      </c>
+      <c r="R4" s="31">
+        <v>5.7357719328453995E-2</v>
+      </c>
+      <c r="S4" s="31">
+        <v>0.28678859664226997</v>
+      </c>
+      <c r="T4" s="31">
+        <v>0.30506801857525023</v>
+      </c>
+      <c r="U4" s="31">
+        <v>0.11812734210692455</v>
+      </c>
+      <c r="V4" s="31">
+        <v>0.11812734210692455</v>
+      </c>
+      <c r="W4" s="31">
+        <v>7.8759319788092377E-2</v>
+      </c>
+      <c r="X4" s="31">
+        <v>3.1503727915236951E-2</v>
+      </c>
+      <c r="Y4" s="31">
+        <v>0.15751863957618475</v>
+      </c>
+      <c r="Z4" s="31">
+        <v>0.17035204037908908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30">
+        <v>14</v>
+      </c>
+      <c r="C5" s="31">
+        <v>0.34088517030620885</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.34088517030620885</v>
+      </c>
+      <c r="E5" s="31">
+        <v>0.20607734542577039</v>
+      </c>
+      <c r="F5" s="31">
+        <v>8.2430938170308166E-2</v>
+      </c>
+      <c r="G5" s="31">
+        <v>0.41215469085154077</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0.43278738883748519</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.1826118330759173</v>
+      </c>
+      <c r="J5" s="31">
+        <v>0.1826118330759173</v>
+      </c>
+      <c r="K5" s="31">
+        <v>0.11733430654736889</v>
+      </c>
+      <c r="L5" s="31">
+        <v>4.6933722618947557E-2</v>
+      </c>
+      <c r="M5" s="31">
+        <v>0.23466861309473777</v>
+      </c>
+      <c r="N5" s="31">
+        <v>0.25098451361873508</v>
+      </c>
+      <c r="O5" s="31">
+        <v>0.25334536391786272</v>
+      </c>
+      <c r="P5" s="31">
+        <v>0.25334536391786272</v>
+      </c>
+      <c r="Q5" s="31">
+        <v>0.15833641389671313</v>
+      </c>
+      <c r="R5" s="31">
+        <v>6.333456555868526E-2</v>
+      </c>
+      <c r="S5" s="31">
+        <v>0.31667282779342626</v>
+      </c>
+      <c r="T5" s="31">
+        <v>0.33581456139269328</v>
+      </c>
+      <c r="U5" s="31">
+        <v>0.13498996822169568</v>
+      </c>
+      <c r="V5" s="31">
+        <v>0.13498996822169568</v>
+      </c>
+      <c r="W5" s="31">
+        <v>8.9350007571831425E-2</v>
+      </c>
+      <c r="X5" s="31">
+        <v>3.5740003028732571E-2</v>
+      </c>
+      <c r="Y5" s="31">
+        <v>0.17870001514366285</v>
+      </c>
+      <c r="Z5" s="31">
+        <v>0.1928241918647402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30">
+        <v>15</v>
+      </c>
+      <c r="C6" s="31">
+        <v>0.37297959555570837</v>
+      </c>
+      <c r="D6" s="31">
+        <v>0.37297959555570837</v>
+      </c>
+      <c r="E6" s="31">
+        <v>0.22280641298931159</v>
+      </c>
+      <c r="F6" s="31">
+        <v>8.9122565195724646E-2</v>
+      </c>
+      <c r="G6" s="31">
+        <v>0.44561282597862317</v>
+      </c>
+      <c r="H6" s="31">
+        <v>0.46631966818466064</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.20527077203822922</v>
+      </c>
+      <c r="J6" s="31">
+        <v>0.20527077203822922</v>
+      </c>
+      <c r="K6" s="31">
+        <v>0.13071766373990495</v>
+      </c>
+      <c r="L6" s="31">
+        <v>5.2287065495961987E-2</v>
+      </c>
+      <c r="M6" s="31">
+        <v>0.26143532747980991</v>
+      </c>
+      <c r="N6" s="31">
+        <v>0.2788329969838958</v>
+      </c>
+      <c r="O6" s="31">
+        <v>0.28134234111565104</v>
+      </c>
+      <c r="P6" s="31">
+        <v>0.28134234111565104</v>
+      </c>
+      <c r="Q6" s="31">
+        <v>0.17395269912062988</v>
+      </c>
+      <c r="R6" s="31">
+        <v>6.9581079648251956E-2</v>
+      </c>
+      <c r="S6" s="31">
+        <v>0.34790539824125977</v>
+      </c>
+      <c r="T6" s="31">
+        <v>0.36774544154318123</v>
+      </c>
+      <c r="U6" s="31">
+        <v>0.15376761844856132</v>
+      </c>
+      <c r="V6" s="31">
+        <v>0.15376761844856132</v>
+      </c>
+      <c r="W6" s="31">
+        <v>0.10099071173125469</v>
+      </c>
+      <c r="X6" s="31">
+        <v>4.039628469250188E-2</v>
+      </c>
+      <c r="Y6" s="31">
+        <v>0.20198142346250939</v>
+      </c>
+      <c r="Z6" s="31">
+        <v>0.2174205760205149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="29"/>
+      <c r="B7" s="30">
+        <v>16</v>
+      </c>
+      <c r="C7" s="31">
+        <v>0.40590286485032145</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.40590286485032145</v>
+      </c>
+      <c r="E7" s="31">
+        <v>0.23955994039648146</v>
+      </c>
+      <c r="F7" s="31">
+        <v>9.5823976158592589E-2</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.47911988079296292</v>
+      </c>
+      <c r="H7" s="31">
+        <v>0.49967163505930923</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.22984150185422531</v>
+      </c>
+      <c r="J7" s="31">
+        <v>0.22984150185422531</v>
+      </c>
+      <c r="K7" s="31">
+        <v>0.14496290751763549</v>
+      </c>
+      <c r="L7" s="31">
+        <v>5.7985163007054197E-2</v>
+      </c>
+      <c r="M7" s="31">
+        <v>0.28992581503527098</v>
+      </c>
+      <c r="N7" s="31">
+        <v>0.30830473406242848</v>
+      </c>
+      <c r="O7" s="31">
+        <v>0.31094663185899651</v>
+      </c>
+      <c r="P7" s="31">
+        <v>0.31094663185899651</v>
+      </c>
+      <c r="Q7" s="31">
+        <v>0.19010575385890205</v>
+      </c>
+      <c r="R7" s="31">
+        <v>7.6042301543560828E-2</v>
+      </c>
+      <c r="S7" s="31">
+        <v>0.3802115077178041</v>
+      </c>
+      <c r="T7" s="31">
+        <v>0.400557726583739</v>
+      </c>
+      <c r="U7" s="31">
+        <v>0.17456098946800941</v>
+      </c>
+      <c r="V7" s="31">
+        <v>0.17456098946800941</v>
+      </c>
+      <c r="W7" s="31">
+        <v>0.11369705502458326</v>
+      </c>
+      <c r="X7" s="31">
+        <v>4.5478822009833303E-2</v>
+      </c>
+      <c r="Y7" s="31">
+        <v>0.22739411004916651</v>
+      </c>
+      <c r="Z7" s="31">
+        <v>0.2441453798977363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30">
+        <v>17</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.43931041752524763</v>
+      </c>
+      <c r="D8" s="31">
+        <v>0.43931041752524763</v>
+      </c>
+      <c r="E8" s="31">
+        <v>0.25615293729640171</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.10246117491856069</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.51230587459280341</v>
+      </c>
+      <c r="H8" s="31">
+        <v>0.53248010431806703</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.25626950146858768</v>
+      </c>
+      <c r="J8" s="31">
+        <v>0.25626950146858768</v>
+      </c>
+      <c r="K8" s="31">
+        <v>0.1599832457702407</v>
+      </c>
+      <c r="L8" s="31">
+        <v>6.3993298308096289E-2</v>
+      </c>
+      <c r="M8" s="31">
+        <v>0.3199664915404814</v>
+      </c>
+      <c r="N8" s="31">
+        <v>0.3391916149673575</v>
+      </c>
+      <c r="O8" s="31">
+        <v>0.34194531751522267</v>
+      </c>
+      <c r="P8" s="31">
+        <v>0.34194531751522267</v>
+      </c>
+      <c r="Q8" s="31">
+        <v>0.20663635589135371</v>
+      </c>
+      <c r="R8" s="31">
+        <v>8.2654542356541488E-2</v>
+      </c>
+      <c r="S8" s="31">
+        <v>0.41327271178270741</v>
+      </c>
+      <c r="T8" s="31">
+        <v>0.43391160779937243</v>
+      </c>
+      <c r="U8" s="31">
+        <v>0.19744414348984035</v>
+      </c>
+      <c r="V8" s="31">
+        <v>0.19744414348984035</v>
+      </c>
+      <c r="W8" s="31">
+        <v>0.12746196303048396</v>
+      </c>
+      <c r="X8" s="31">
+        <v>5.0984785212193587E-2</v>
+      </c>
+      <c r="Y8" s="31">
+        <v>0.25492392606096792</v>
+      </c>
+      <c r="Z8" s="31">
+        <v>0.27295251423225325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30">
+        <v>18</v>
+      </c>
+      <c r="C9" s="31">
+        <v>0.47283666905654426</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0.47283666905654426</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.2724074242967654</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.10896296971870617</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0.5448148485935308</v>
+      </c>
+      <c r="H9" s="31">
+        <v>0.56440535977475093</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.28444759676866466</v>
+      </c>
+      <c r="J9" s="31">
+        <v>0.28444759676866466</v>
+      </c>
+      <c r="K9" s="31">
+        <v>0.17566418191339275</v>
+      </c>
+      <c r="L9" s="31">
+        <v>7.0265672765357098E-2</v>
+      </c>
+      <c r="M9" s="31">
+        <v>0.35132836382678551</v>
+      </c>
+      <c r="N9" s="31">
+        <v>0.37123241188241834</v>
+      </c>
+      <c r="O9" s="31">
+        <v>0.37407280623808481</v>
+      </c>
+      <c r="P9" s="31">
+        <v>0.37407280623808481</v>
+      </c>
+      <c r="Q9" s="31">
+        <v>0.22336925491177653</v>
+      </c>
+      <c r="R9" s="31">
+        <v>8.9347701964710619E-2</v>
+      </c>
+      <c r="S9" s="31">
+        <v>0.44673850982355306</v>
+      </c>
+      <c r="T9" s="31">
+        <v>0.46744385435332725</v>
+      </c>
+      <c r="U9" s="31">
+        <v>0.22245591706785262</v>
+      </c>
+      <c r="V9" s="31">
+        <v>0.22245591706785262</v>
+      </c>
+      <c r="W9" s="31">
+        <v>0.14225184079766034</v>
+      </c>
+      <c r="X9" s="31">
+        <v>5.6900736319064144E-2</v>
+      </c>
+      <c r="Y9" s="31">
+        <v>0.28450368159532069</v>
+      </c>
+      <c r="Z9" s="31">
+        <v>0.30373896298734987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="29"/>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="29"/>
+      <c r="B12" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q12" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="U12" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="V12" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="X12" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y12" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z12" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="29"/>
+      <c r="B13" s="32">
+        <v>12</v>
+      </c>
+      <c r="C13" s="23">
+        <f>ROUND(C3,5)</f>
+        <v>0.29550999999999999</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" ref="D13:Z19" si="0">ROUND(D3,5)</f>
+        <v>0.29550999999999999</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18447</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="0"/>
+        <v>7.3789999999999994E-2</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.36895</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.39088000000000001</v>
+      </c>
+      <c r="I13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15115000000000001</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15115000000000001</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="0"/>
+        <v>9.9610000000000004E-2</v>
+      </c>
+      <c r="L13" s="23">
+        <f t="shared" si="0"/>
+        <v>3.984E-2</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19921</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21461</v>
+      </c>
+      <c r="O13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21404999999999999</v>
+      </c>
+      <c r="P13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21404999999999999</v>
+      </c>
+      <c r="Q13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13772999999999999</v>
+      </c>
+      <c r="R13" s="23">
+        <f t="shared" si="0"/>
+        <v>5.509E-2</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27545999999999998</v>
+      </c>
+      <c r="T13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.29453000000000001</v>
+      </c>
+      <c r="U13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10306</v>
+      </c>
+      <c r="V13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10306</v>
+      </c>
+      <c r="W13" s="23">
+        <f t="shared" si="0"/>
+        <v>6.9180000000000005E-2</v>
+      </c>
+      <c r="X13" s="23">
+        <f t="shared" si="0"/>
+        <v>2.767E-2</v>
+      </c>
+      <c r="Y13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13836999999999999</v>
+      </c>
+      <c r="Z13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14996000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="29"/>
+      <c r="B14" s="32">
+        <v>13</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" ref="C14:R19" si="1">ROUND(C4,5)</f>
+        <v>0.30992999999999998</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.30992999999999998</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.18956000000000001</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>7.5819999999999999E-2</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.37911</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.39945000000000003</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.16187000000000001</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.16187000000000001</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10487</v>
+      </c>
+      <c r="L14" s="23">
+        <f t="shared" si="1"/>
+        <v>4.1950000000000001E-2</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.20974000000000001</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.22491</v>
+      </c>
+      <c r="O14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.22711000000000001</v>
+      </c>
+      <c r="P14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.22711000000000001</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="1"/>
+        <v>0.14338999999999999</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.7360000000000001E-2</v>
+      </c>
+      <c r="S14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28678999999999999</v>
+      </c>
+      <c r="T14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.30507000000000001</v>
+      </c>
+      <c r="U14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11813</v>
+      </c>
+      <c r="V14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11813</v>
+      </c>
+      <c r="W14" s="23">
+        <f t="shared" si="0"/>
+        <v>7.8759999999999997E-2</v>
+      </c>
+      <c r="X14" s="23">
+        <f t="shared" si="0"/>
+        <v>3.15E-2</v>
+      </c>
+      <c r="Y14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15751999999999999</v>
+      </c>
+      <c r="Z14" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="29"/>
+      <c r="B15" s="32">
+        <v>14</v>
+      </c>
+      <c r="C15" s="23">
+        <f t="shared" si="1"/>
+        <v>0.34089000000000003</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.34089000000000003</v>
+      </c>
+      <c r="E15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20608000000000001</v>
+      </c>
+      <c r="F15" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2430000000000003E-2</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.41215000000000002</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.43279000000000001</v>
+      </c>
+      <c r="I15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18260999999999999</v>
+      </c>
+      <c r="J15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.18260999999999999</v>
+      </c>
+      <c r="K15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11733</v>
+      </c>
+      <c r="L15" s="23">
+        <f t="shared" si="0"/>
+        <v>4.6929999999999999E-2</v>
+      </c>
+      <c r="M15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23466999999999999</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25097999999999998</v>
+      </c>
+      <c r="O15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25335000000000002</v>
+      </c>
+      <c r="P15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25335000000000002</v>
+      </c>
+      <c r="Q15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15834000000000001</v>
+      </c>
+      <c r="R15" s="23">
+        <f t="shared" si="0"/>
+        <v>6.3329999999999997E-2</v>
+      </c>
+      <c r="S15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31667000000000001</v>
+      </c>
+      <c r="T15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.33581</v>
+      </c>
+      <c r="U15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13499</v>
+      </c>
+      <c r="V15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13499</v>
+      </c>
+      <c r="W15" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9349999999999999E-2</v>
+      </c>
+      <c r="X15" s="23">
+        <f t="shared" si="0"/>
+        <v>3.5740000000000001E-2</v>
+      </c>
+      <c r="Y15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1787</v>
+      </c>
+      <c r="Z15" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19281999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="29"/>
+      <c r="B16" s="32">
+        <v>15</v>
+      </c>
+      <c r="C16" s="23">
+        <f t="shared" si="1"/>
+        <v>0.37297999999999998</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.37297999999999998</v>
+      </c>
+      <c r="E16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22281000000000001</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9120000000000005E-2</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.44561000000000001</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.46632000000000001</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20527000000000001</v>
+      </c>
+      <c r="J16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20527000000000001</v>
+      </c>
+      <c r="K16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13072</v>
+      </c>
+      <c r="L16" s="23">
+        <f t="shared" si="0"/>
+        <v>5.2290000000000003E-2</v>
+      </c>
+      <c r="M16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.26144000000000001</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27883000000000002</v>
+      </c>
+      <c r="O16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28133999999999998</v>
+      </c>
+      <c r="P16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28133999999999998</v>
+      </c>
+      <c r="Q16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17394999999999999</v>
+      </c>
+      <c r="R16" s="23">
+        <f t="shared" si="0"/>
+        <v>6.9580000000000003E-2</v>
+      </c>
+      <c r="S16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.34791</v>
+      </c>
+      <c r="T16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.36775000000000002</v>
+      </c>
+      <c r="U16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15376999999999999</v>
+      </c>
+      <c r="V16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15376999999999999</v>
+      </c>
+      <c r="W16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10099</v>
+      </c>
+      <c r="X16" s="23">
+        <f t="shared" si="0"/>
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="Y16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20197999999999999</v>
+      </c>
+      <c r="Z16" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" s="29"/>
+      <c r="B17" s="32">
+        <v>16</v>
+      </c>
+      <c r="C17" s="23">
+        <f t="shared" si="1"/>
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23956</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="0"/>
+        <v>9.5820000000000002E-2</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.47911999999999999</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.49967</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22983999999999999</v>
+      </c>
+      <c r="J17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22983999999999999</v>
+      </c>
+      <c r="K17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14496000000000001</v>
+      </c>
+      <c r="L17" s="23">
+        <f t="shared" si="0"/>
+        <v>5.799E-2</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28993000000000002</v>
+      </c>
+      <c r="N17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.30830000000000002</v>
+      </c>
+      <c r="O17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31095</v>
+      </c>
+      <c r="P17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31095</v>
+      </c>
+      <c r="Q17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19011</v>
+      </c>
+      <c r="R17" s="23">
+        <f t="shared" si="0"/>
+        <v>7.6039999999999996E-2</v>
+      </c>
+      <c r="S17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.38020999999999999</v>
+      </c>
+      <c r="T17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.40056000000000003</v>
+      </c>
+      <c r="U17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17455999999999999</v>
+      </c>
+      <c r="V17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17455999999999999</v>
+      </c>
+      <c r="W17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1137</v>
+      </c>
+      <c r="X17" s="23">
+        <f t="shared" si="0"/>
+        <v>4.548E-2</v>
+      </c>
+      <c r="Y17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22739000000000001</v>
+      </c>
+      <c r="Z17" s="23">
+        <f t="shared" si="0"/>
+        <v>0.24415000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" s="29"/>
+      <c r="B18" s="32">
+        <v>17</v>
+      </c>
+      <c r="C18" s="23">
+        <f t="shared" si="1"/>
+        <v>0.43930999999999998</v>
+      </c>
+      <c r="D18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.43930999999999998</v>
+      </c>
+      <c r="E18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25614999999999999</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10246</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.51231000000000004</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.53247999999999995</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25627</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25627</v>
+      </c>
+      <c r="K18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15998000000000001</v>
+      </c>
+      <c r="L18" s="23">
+        <f t="shared" si="0"/>
+        <v>6.3990000000000005E-2</v>
+      </c>
+      <c r="M18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.31996999999999998</v>
+      </c>
+      <c r="N18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.33918999999999999</v>
+      </c>
+      <c r="O18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.34194999999999998</v>
+      </c>
+      <c r="P18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.34194999999999998</v>
+      </c>
+      <c r="Q18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20663999999999999</v>
+      </c>
+      <c r="R18" s="23">
+        <f t="shared" si="0"/>
+        <v>8.2650000000000001E-2</v>
+      </c>
+      <c r="S18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.41327000000000003</v>
+      </c>
+      <c r="T18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.43391000000000002</v>
+      </c>
+      <c r="U18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19744</v>
+      </c>
+      <c r="V18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.19744</v>
+      </c>
+      <c r="W18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.12745999999999999</v>
+      </c>
+      <c r="X18" s="23">
+        <f t="shared" si="0"/>
+        <v>5.0979999999999998E-2</v>
+      </c>
+      <c r="Y18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25491999999999998</v>
+      </c>
+      <c r="Z18" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27295000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19" s="29"/>
+      <c r="B19" s="32">
+        <v>18</v>
+      </c>
+      <c r="C19" s="23">
+        <f t="shared" si="1"/>
+        <v>0.47283999999999998</v>
+      </c>
+      <c r="D19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.47283999999999998</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27240999999999999</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10896</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.54481000000000002</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.56440999999999997</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28444999999999998</v>
+      </c>
+      <c r="J19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28444999999999998</v>
+      </c>
+      <c r="K19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.17566000000000001</v>
+      </c>
+      <c r="L19" s="23">
+        <f t="shared" si="0"/>
+        <v>7.0269999999999999E-2</v>
+      </c>
+      <c r="M19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.35132999999999998</v>
+      </c>
+      <c r="N19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.37123</v>
+      </c>
+      <c r="O19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.37407000000000001</v>
+      </c>
+      <c r="P19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.37407000000000001</v>
+      </c>
+      <c r="Q19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22337000000000001</v>
+      </c>
+      <c r="R19" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9349999999999999E-2</v>
+      </c>
+      <c r="S19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.44674000000000003</v>
+      </c>
+      <c r="T19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.46744000000000002</v>
+      </c>
+      <c r="U19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22245999999999999</v>
+      </c>
+      <c r="V19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.22245999999999999</v>
+      </c>
+      <c r="W19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.14224999999999999</v>
+      </c>
+      <c r="X19" s="23">
+        <f t="shared" si="0"/>
+        <v>5.6899999999999999E-2</v>
+      </c>
+      <c r="Y19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.28449999999999998</v>
+      </c>
+      <c r="Z19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.30374000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20" s="29"/>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21" s="29"/>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add proper debut rates
</commit_message>
<xml_diff>
--- a/data_prep/input_data.xlsx
+++ b/data_prep/input_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="12435" windowHeight="10485" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="4" r:id="rId1"/>
@@ -16,9 +16,11 @@
     <sheet name="Abused Depression" sheetId="7" r:id="rId7"/>
     <sheet name="Not Abused Condom Rates" sheetId="8" r:id="rId8"/>
     <sheet name="Abused Condom Rates" sheetId="9" r:id="rId9"/>
+    <sheet name="Not Abused Debut" sheetId="10" r:id="rId10"/>
+    <sheet name="Abused Debut" sheetId="11" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="CurrYear">[1]Results!$B$3</definedName>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="72">
   <si>
     <t>Age</t>
   </si>
@@ -547,7 +549,7 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="174" fontId="2" fillId="0" borderId="4" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -594,6 +596,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Bold 11" xfId="2"/>
@@ -1395,6 +1400,1447 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="36"/>
+      <c r="B2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="36"/>
+      <c r="B3" s="38">
+        <v>13</v>
+      </c>
+      <c r="C3" s="23">
+        <v>3.409219227467352E-2</v>
+      </c>
+      <c r="D3" s="23">
+        <v>3.409219227467352E-2</v>
+      </c>
+      <c r="E3" s="23">
+        <v>2.0466978028009713E-2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>8.1867912112038848E-3</v>
+      </c>
+      <c r="G3" s="23">
+        <v>4.0933956056019426E-2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>3.4723429533357553E-2</v>
+      </c>
+      <c r="I3" s="23">
+        <v>3.8530970774725296E-2</v>
+      </c>
+      <c r="J3" s="23">
+        <v>3.8530970774725296E-2</v>
+      </c>
+      <c r="K3" s="23">
+        <v>2.3110450364287813E-2</v>
+      </c>
+      <c r="L3" s="23">
+        <v>9.2441801457151251E-3</v>
+      </c>
+      <c r="M3" s="23">
+        <v>4.6220900728575626E-2</v>
+      </c>
+      <c r="N3" s="23">
+        <v>3.9241055741568859E-2</v>
+      </c>
+      <c r="O3" s="23">
+        <v>8.9643139931506508E-2</v>
+      </c>
+      <c r="P3" s="23">
+        <v>8.9643139931506508E-2</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>5.3202503998716094E-2</v>
+      </c>
+      <c r="R3" s="23">
+        <v>2.128100159948644E-2</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.10640500799743219</v>
+      </c>
+      <c r="T3" s="23">
+        <v>9.1205814451810446E-2</v>
+      </c>
+      <c r="U3" s="23">
+        <v>0.10056160845706009</v>
+      </c>
+      <c r="V3" s="23">
+        <v>0.10056160845706009</v>
+      </c>
+      <c r="W3" s="23">
+        <v>5.9548984205744247E-2</v>
+      </c>
+      <c r="X3" s="23">
+        <v>2.3819593682297701E-2</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>0.11909796841148849</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>0.10229322865649333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="B4" s="38">
+        <v>14</v>
+      </c>
+      <c r="C4" s="23">
+        <v>1.1908785249521138E-2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1.1908785249521138E-2</v>
+      </c>
+      <c r="E4" s="23">
+        <v>7.0811837968055048E-3</v>
+      </c>
+      <c r="F4" s="23">
+        <v>2.8324735187222026E-3</v>
+      </c>
+      <c r="G4" s="23">
+        <v>1.416236759361101E-2</v>
+      </c>
+      <c r="H4" s="23">
+        <v>1.2118590369800647E-2</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1.3375977201265044E-2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>1.3375977201265044E-2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>7.9365602598665715E-3</v>
+      </c>
+      <c r="L4" s="23">
+        <v>3.17462410394663E-3</v>
+      </c>
+      <c r="M4" s="23">
+        <v>1.5873120519733143E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <v>1.360893240786918E-2</v>
+      </c>
+      <c r="O4" s="23">
+        <v>2.8931258503432339E-2</v>
+      </c>
+      <c r="P4" s="23">
+        <v>2.8931258503432339E-2</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>1.6754762917791252E-2</v>
+      </c>
+      <c r="R4" s="23">
+        <v>6.7019051671164988E-3</v>
+      </c>
+      <c r="S4" s="23">
+        <v>3.3509525835582504E-2</v>
+      </c>
+      <c r="T4" s="23">
+        <v>2.9368795213074311E-2</v>
+      </c>
+      <c r="U4" s="23">
+        <v>3.1942169375229881E-2</v>
+      </c>
+      <c r="V4" s="23">
+        <v>3.1942169375229881E-2</v>
+      </c>
+      <c r="W4" s="23">
+        <v>1.8404713356731668E-2</v>
+      </c>
+      <c r="X4" s="23">
+        <v>7.3618853426926679E-3</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>3.6809426713463336E-2</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>3.2409823295534837E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="B5" s="38">
+        <v>15</v>
+      </c>
+      <c r="C5" s="23">
+        <v>1.5802488739393883E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1.5802488739393883E-2</v>
+      </c>
+      <c r="E5" s="23">
+        <v>9.3426614764174146E-3</v>
+      </c>
+      <c r="F5" s="23">
+        <v>3.7370645905669669E-3</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1.8685322952834829E-2</v>
+      </c>
+      <c r="H5" s="23">
+        <v>1.6072354222944812E-2</v>
+      </c>
+      <c r="I5" s="23">
+        <v>1.7683341467696803E-2</v>
+      </c>
+      <c r="J5" s="23">
+        <v>1.7683341467696803E-2</v>
+      </c>
+      <c r="K5" s="23">
+        <v>1.0425098064409919E-2</v>
+      </c>
+      <c r="L5" s="23">
+        <v>4.1700392257639669E-3</v>
+      </c>
+      <c r="M5" s="23">
+        <v>2.0850196128819838E-2</v>
+      </c>
+      <c r="N5" s="23">
+        <v>1.7980609091881906E-2</v>
+      </c>
+      <c r="O5" s="23">
+        <v>3.6676126782527421E-2</v>
+      </c>
+      <c r="P5" s="23">
+        <v>3.6676126782527421E-2</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>2.0957580919364352E-2</v>
+      </c>
+      <c r="R5" s="23">
+        <v>8.3830323677457387E-3</v>
+      </c>
+      <c r="S5" s="23">
+        <v>4.1915161838728704E-2</v>
+      </c>
+      <c r="T5" s="23">
+        <v>3.7184077354085188E-2</v>
+      </c>
+      <c r="U5" s="23">
+        <v>4.014070826591945E-2</v>
+      </c>
+      <c r="V5" s="23">
+        <v>4.014070826591945E-2</v>
+      </c>
+      <c r="W5" s="23">
+        <v>2.2791924985128498E-2</v>
+      </c>
+      <c r="X5" s="23">
+        <v>9.1167699940514005E-3</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>4.5583849970256995E-2</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>4.0672266081934388E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="B11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="S11" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="X11" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z11" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="B12" s="39">
+        <v>13</v>
+      </c>
+      <c r="C12" s="23">
+        <f>ROUND(C3,5)</f>
+        <v>3.4090000000000002E-2</v>
+      </c>
+      <c r="D12" s="23">
+        <f t="shared" ref="D12:Z12" si="0">ROUND(D3,5)</f>
+        <v>3.4090000000000002E-2</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>2.0469999999999999E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.1899999999999994E-3</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="0"/>
+        <v>4.0930000000000001E-2</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.4720000000000001E-2</v>
+      </c>
+      <c r="I12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.8530000000000002E-2</v>
+      </c>
+      <c r="J12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.8530000000000002E-2</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="0"/>
+        <v>2.3109999999999999E-2</v>
+      </c>
+      <c r="L12" s="23">
+        <f t="shared" si="0"/>
+        <v>9.2399999999999999E-3</v>
+      </c>
+      <c r="M12" s="23">
+        <f t="shared" si="0"/>
+        <v>4.6219999999999997E-2</v>
+      </c>
+      <c r="N12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.9239999999999997E-2</v>
+      </c>
+      <c r="O12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9639999999999997E-2</v>
+      </c>
+      <c r="P12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.9639999999999997E-2</v>
+      </c>
+      <c r="Q12" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="R12" s="23">
+        <f t="shared" si="0"/>
+        <v>2.128E-2</v>
+      </c>
+      <c r="S12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10641</v>
+      </c>
+      <c r="T12" s="23">
+        <f t="shared" si="0"/>
+        <v>9.1209999999999999E-2</v>
+      </c>
+      <c r="U12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10056</v>
+      </c>
+      <c r="V12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10056</v>
+      </c>
+      <c r="W12" s="23">
+        <f t="shared" si="0"/>
+        <v>5.9549999999999999E-2</v>
+      </c>
+      <c r="X12" s="23">
+        <f t="shared" si="0"/>
+        <v>2.3820000000000001E-2</v>
+      </c>
+      <c r="Y12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1191</v>
+      </c>
+      <c r="Z12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10229000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="B13" s="39">
+        <v>14</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" ref="C13:Z13" si="1">ROUND(C4,5)</f>
+        <v>1.191E-2</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.191E-2</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="1"/>
+        <v>7.0800000000000004E-3</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.8300000000000001E-3</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.4160000000000001E-2</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.2120000000000001E-2</v>
+      </c>
+      <c r="I13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.338E-2</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.338E-2</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="1"/>
+        <v>7.9399999999999991E-3</v>
+      </c>
+      <c r="L13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.1700000000000001E-3</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.5869999999999999E-2</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.3610000000000001E-2</v>
+      </c>
+      <c r="O13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.8930000000000001E-2</v>
+      </c>
+      <c r="P13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.8930000000000001E-2</v>
+      </c>
+      <c r="Q13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="R13" s="23">
+        <f t="shared" si="1"/>
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.3509999999999998E-2</v>
+      </c>
+      <c r="T13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.937E-2</v>
+      </c>
+      <c r="U13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.1940000000000003E-2</v>
+      </c>
+      <c r="V13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.1940000000000003E-2</v>
+      </c>
+      <c r="W13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.84E-2</v>
+      </c>
+      <c r="X13" s="23">
+        <f t="shared" si="1"/>
+        <v>7.3600000000000002E-3</v>
+      </c>
+      <c r="Y13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.6810000000000002E-2</v>
+      </c>
+      <c r="Z13" s="23">
+        <f t="shared" si="1"/>
+        <v>3.2410000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="B14" s="39">
+        <v>15</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" ref="C14:Z14" si="2">ROUND(C5,5)</f>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="2"/>
+        <v>9.3399999999999993E-3</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="2"/>
+        <v>3.7399999999999998E-3</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.8689999999999998E-2</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.6070000000000001E-2</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.7680000000000001E-2</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.7680000000000001E-2</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.043E-2</v>
+      </c>
+      <c r="L14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.1700000000000001E-3</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="2"/>
+        <v>2.085E-2</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="2"/>
+        <v>1.7979999999999999E-2</v>
+      </c>
+      <c r="O14" s="23">
+        <f t="shared" si="2"/>
+        <v>3.6679999999999997E-2</v>
+      </c>
+      <c r="P14" s="23">
+        <f t="shared" si="2"/>
+        <v>3.6679999999999997E-2</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="2"/>
+        <v>2.0959999999999999E-2</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" si="2"/>
+        <v>8.3800000000000003E-3</v>
+      </c>
+      <c r="S14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.1919999999999999E-2</v>
+      </c>
+      <c r="T14" s="23">
+        <f t="shared" si="2"/>
+        <v>3.7179999999999998E-2</v>
+      </c>
+      <c r="U14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.0140000000000002E-2</v>
+      </c>
+      <c r="V14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.0140000000000002E-2</v>
+      </c>
+      <c r="W14" s="23">
+        <f t="shared" si="2"/>
+        <v>2.2790000000000001E-2</v>
+      </c>
+      <c r="X14" s="23">
+        <f t="shared" si="2"/>
+        <v>9.1199999999999996E-3</v>
+      </c>
+      <c r="Y14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.5580000000000002E-2</v>
+      </c>
+      <c r="Z14" s="23">
+        <f t="shared" si="2"/>
+        <v>4.0669999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:Z5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" s="39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="B2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="U2" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" s="40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="B3" s="40">
+        <v>13</v>
+      </c>
+      <c r="C3" s="23">
+        <v>5.3403329799824227E-2</v>
+      </c>
+      <c r="D3" s="23">
+        <v>5.3403329799824227E-2</v>
+      </c>
+      <c r="E3" s="23">
+        <v>3.1932147751673079E-2</v>
+      </c>
+      <c r="F3" s="23">
+        <v>1.2772859100669233E-2</v>
+      </c>
+      <c r="G3" s="23">
+        <v>6.3864295503346158E-2</v>
+      </c>
+      <c r="H3" s="23">
+        <v>5.4371996995758107E-2</v>
+      </c>
+      <c r="I3" s="23">
+        <v>5.3403329799824227E-2</v>
+      </c>
+      <c r="J3" s="23">
+        <v>5.3403329799824227E-2</v>
+      </c>
+      <c r="K3" s="23">
+        <v>3.5945436605017998E-2</v>
+      </c>
+      <c r="L3" s="23">
+        <v>1.43781746420072E-2</v>
+      </c>
+      <c r="M3" s="23">
+        <v>7.1890873210035997E-2</v>
+      </c>
+      <c r="N3" s="23">
+        <v>0.15407385387469932</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0.1359903512204356</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0.1359903512204356</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>7.9948140361099845E-2</v>
+      </c>
+      <c r="R3" s="23">
+        <v>3.1979256144439937E-2</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.15989628072219969</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0.1382382731724941</v>
+      </c>
+      <c r="U3" s="23">
+        <v>0.15161373035576886</v>
+      </c>
+      <c r="V3" s="23">
+        <v>0.15161373035576886</v>
+      </c>
+      <c r="W3" s="23">
+        <v>8.8850625174313455E-2</v>
+      </c>
+      <c r="X3" s="23">
+        <v>3.5540250069725381E-2</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>0.17770125034862691</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>0.15407385387469932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="B4" s="40">
+        <v>14</v>
+      </c>
+      <c r="C4" s="23">
+        <v>1.8154643812736536E-2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1.8154643812736536E-2</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1.0695296583093421E-2</v>
+      </c>
+      <c r="F4" s="23">
+        <v>4.2781186332373679E-3</v>
+      </c>
+      <c r="G4" s="23">
+        <v>2.1390593166186841E-2</v>
+      </c>
+      <c r="H4" s="23">
+        <v>1.8458609239168977E-2</v>
+      </c>
+      <c r="I4" s="23">
+        <v>1.8154643812736536E-2</v>
+      </c>
+      <c r="J4" s="23">
+        <v>1.8154643812736536E-2</v>
+      </c>
+      <c r="K4" s="23">
+        <v>1.1902091189944085E-2</v>
+      </c>
+      <c r="L4" s="23">
+        <v>4.760836475977635E-3</v>
+      </c>
+      <c r="M4" s="23">
+        <v>2.380418237988817E-2</v>
+      </c>
+      <c r="N4" s="23">
+        <v>4.5174306657326468E-2</v>
+      </c>
+      <c r="O4" s="23">
+        <v>4.0981458556913097E-2</v>
+      </c>
+      <c r="P4" s="23">
+        <v>4.0981458556913097E-2</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>2.3232493578632704E-2</v>
+      </c>
+      <c r="R4" s="23">
+        <v>9.2929974314530858E-3</v>
+      </c>
+      <c r="S4" s="23">
+        <v>4.6464987157265408E-2</v>
+      </c>
+      <c r="T4" s="23">
+        <v>4.1517945226252378E-2</v>
+      </c>
+      <c r="U4" s="23">
+        <v>4.4620326010010342E-2</v>
+      </c>
+      <c r="V4" s="23">
+        <v>4.4620326010010342E-2</v>
+      </c>
+      <c r="W4" s="23">
+        <v>2.5117600112294775E-2</v>
+      </c>
+      <c r="X4" s="23">
+        <v>1.0047040044917917E-2</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>5.0235200224589549E-2</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>4.5174306657326468E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="B5" s="40">
+        <v>15</v>
+      </c>
+      <c r="C5" s="23">
+        <v>2.3705268239493482E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2.3705268239493482E-2</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1.3845356862020493E-2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>5.5381427448081971E-3</v>
+      </c>
+      <c r="G5" s="23">
+        <v>2.7690713724040986E-2</v>
+      </c>
+      <c r="H5" s="23">
+        <v>2.4082851103374076E-2</v>
+      </c>
+      <c r="I5" s="23">
+        <v>2.3705268239493482E-2</v>
+      </c>
+      <c r="J5" s="23">
+        <v>2.3705268239493482E-2</v>
+      </c>
+      <c r="K5" s="23">
+        <v>1.5306722831069375E-2</v>
+      </c>
+      <c r="L5" s="23">
+        <v>6.1226891324277499E-3</v>
+      </c>
+      <c r="M5" s="23">
+        <v>3.061344566213875E-2</v>
+      </c>
+      <c r="N5" s="23">
+        <v>5.444714348891147E-2</v>
+      </c>
+      <c r="O5" s="23">
+        <v>5.0085930825912756E-2</v>
+      </c>
+      <c r="P5" s="23">
+        <v>5.0085930825912756E-2</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>2.7877315464450089E-2</v>
+      </c>
+      <c r="R5" s="23">
+        <v>1.1150926185780036E-2</v>
+      </c>
+      <c r="S5" s="23">
+        <v>5.5754630928900178E-2</v>
+      </c>
+      <c r="T5" s="23">
+        <v>5.0653351570318417E-2</v>
+      </c>
+      <c r="U5" s="23">
+        <v>5.3880765331910302E-2</v>
+      </c>
+      <c r="V5" s="23">
+        <v>5.3880765331910302E-2</v>
+      </c>
+      <c r="W5" s="23">
+        <v>2.97364114096446E-2</v>
+      </c>
+      <c r="X5" s="23">
+        <v>1.1894564563857839E-2</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>5.9472822819289201E-2</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>5.444714348891147E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="B11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="S11" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="U11" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="X11" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y11" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z11" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="B12" s="39">
+        <v>13</v>
+      </c>
+      <c r="C12" s="23">
+        <f>ROUND(C3,5)</f>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="D12" s="23">
+        <f t="shared" ref="D12:Z12" si="0">ROUND(D3,5)</f>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.193E-2</v>
+      </c>
+      <c r="F12" s="23">
+        <f t="shared" si="0"/>
+        <v>1.277E-2</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="0"/>
+        <v>6.386E-2</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="0"/>
+        <v>5.4370000000000002E-2</v>
+      </c>
+      <c r="I12" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="J12" s="23">
+        <f t="shared" si="0"/>
+        <v>5.3400000000000003E-2</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.5950000000000003E-2</v>
+      </c>
+      <c r="L12" s="23">
+        <f t="shared" si="0"/>
+        <v>1.438E-2</v>
+      </c>
+      <c r="M12" s="23">
+        <f t="shared" si="0"/>
+        <v>7.1889999999999996E-2</v>
+      </c>
+      <c r="N12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15407000000000001</v>
+      </c>
+      <c r="O12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13599</v>
+      </c>
+      <c r="P12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13599</v>
+      </c>
+      <c r="Q12" s="23">
+        <f t="shared" si="0"/>
+        <v>7.9949999999999993E-2</v>
+      </c>
+      <c r="R12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.1980000000000001E-2</v>
+      </c>
+      <c r="S12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15989999999999999</v>
+      </c>
+      <c r="T12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.13824</v>
+      </c>
+      <c r="U12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15160999999999999</v>
+      </c>
+      <c r="V12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15160999999999999</v>
+      </c>
+      <c r="W12" s="23">
+        <f t="shared" si="0"/>
+        <v>8.8849999999999998E-2</v>
+      </c>
+      <c r="X12" s="23">
+        <f t="shared" si="0"/>
+        <v>3.5540000000000002E-2</v>
+      </c>
+      <c r="Y12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.1777</v>
+      </c>
+      <c r="Z12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.15407000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="B13" s="39">
+        <v>14</v>
+      </c>
+      <c r="C13" s="23">
+        <f t="shared" ref="C13:Z14" si="1">ROUND(C4,5)</f>
+        <v>1.8149999999999999E-2</v>
+      </c>
+      <c r="D13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8149999999999999E-2</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.28E-3</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.1389999999999999E-2</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8460000000000001E-2</v>
+      </c>
+      <c r="I13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8149999999999999E-2</v>
+      </c>
+      <c r="J13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8149999999999999E-2</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="L13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.7600000000000003E-3</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.5170000000000002E-2</v>
+      </c>
+      <c r="O13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.0980000000000003E-2</v>
+      </c>
+      <c r="P13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.0980000000000003E-2</v>
+      </c>
+      <c r="Q13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3230000000000001E-2</v>
+      </c>
+      <c r="R13" s="23">
+        <f t="shared" si="1"/>
+        <v>9.2899999999999996E-3</v>
+      </c>
+      <c r="S13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.6460000000000001E-2</v>
+      </c>
+      <c r="T13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.1520000000000001E-2</v>
+      </c>
+      <c r="U13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.462E-2</v>
+      </c>
+      <c r="V13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.462E-2</v>
+      </c>
+      <c r="W13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.512E-2</v>
+      </c>
+      <c r="X13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.005E-2</v>
+      </c>
+      <c r="Y13" s="23">
+        <f t="shared" si="1"/>
+        <v>5.024E-2</v>
+      </c>
+      <c r="Z13" s="23">
+        <f t="shared" si="1"/>
+        <v>4.5170000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="B14" s="39">
+        <v>15</v>
+      </c>
+      <c r="C14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3709999999999998E-2</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3709999999999998E-2</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.3849999999999999E-2</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.5399999999999998E-3</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.7689999999999999E-2</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.4080000000000001E-2</v>
+      </c>
+      <c r="I14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3709999999999998E-2</v>
+      </c>
+      <c r="J14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.3709999999999998E-2</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.5310000000000001E-2</v>
+      </c>
+      <c r="L14" s="23">
+        <f t="shared" si="1"/>
+        <v>6.1199999999999996E-3</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="1"/>
+        <v>3.0609999999999998E-2</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.4449999999999998E-2</v>
+      </c>
+      <c r="O14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.0090000000000003E-2</v>
+      </c>
+      <c r="P14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.0090000000000003E-2</v>
+      </c>
+      <c r="Q14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.7879999999999999E-2</v>
+      </c>
+      <c r="R14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.115E-2</v>
+      </c>
+      <c r="S14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.5750000000000001E-2</v>
+      </c>
+      <c r="T14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.0650000000000001E-2</v>
+      </c>
+      <c r="U14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.3879999999999997E-2</v>
+      </c>
+      <c r="V14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.3879999999999997E-2</v>
+      </c>
+      <c r="W14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.9739999999999999E-2</v>
+      </c>
+      <c r="X14" s="23">
+        <f t="shared" si="1"/>
+        <v>1.189E-2</v>
+      </c>
+      <c r="Y14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.9470000000000002E-2</v>
+      </c>
+      <c r="Z14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.4449999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X182"/>
@@ -20667,8 +22113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>